<commit_message>
refactor data and add XLSX diff script
</commit_message>
<xml_diff>
--- a/inch_taps_drills.xlsx
+++ b/inch_taps_drills.xlsx
@@ -699,8 +699,6 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="n"/>
-      <c r="B6" s="4" t="n"/>
       <c r="C6" s="4" t="inlineStr">
         <is>
           <t>72</t>
@@ -731,10 +729,6 @@
           <t>.0635</t>
         </is>
       </c>
-      <c r="I6" s="4" t="n"/>
-      <c r="J6" s="4" t="n"/>
-      <c r="K6" s="4" t="n"/>
-      <c r="L6" s="4" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -799,8 +793,6 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n"/>
-      <c r="B8" s="3" t="n"/>
       <c r="C8" s="3" t="inlineStr">
         <is>
           <t>64</t>
@@ -831,10 +823,6 @@
           <t>.0760</t>
         </is>
       </c>
-      <c r="I8" s="3" t="n"/>
-      <c r="J8" s="3" t="n"/>
-      <c r="K8" s="3" t="n"/>
-      <c r="L8" s="3" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -899,8 +887,6 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="n"/>
-      <c r="B10" s="4" t="n"/>
       <c r="C10" s="4" t="inlineStr">
         <is>
           <t>56</t>
@@ -931,10 +917,6 @@
           <t>.0890</t>
         </is>
       </c>
-      <c r="I10" s="4" t="n"/>
-      <c r="J10" s="4" t="n"/>
-      <c r="K10" s="4" t="n"/>
-      <c r="L10" s="4" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -999,8 +981,6 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n"/>
-      <c r="B12" s="3" t="n"/>
       <c r="C12" s="3" t="inlineStr">
         <is>
           <t>48</t>
@@ -1031,10 +1011,6 @@
           <t>.0980</t>
         </is>
       </c>
-      <c r="I12" s="3" t="n"/>
-      <c r="J12" s="3" t="n"/>
-      <c r="K12" s="3" t="n"/>
-      <c r="L12" s="3" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
@@ -1099,8 +1075,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="n"/>
-      <c r="B14" s="4" t="n"/>
       <c r="C14" s="4" t="inlineStr">
         <is>
           <t>44</t>
@@ -1131,10 +1105,6 @@
           <t>.1100</t>
         </is>
       </c>
-      <c r="I14" s="4" t="n"/>
-      <c r="J14" s="4" t="n"/>
-      <c r="K14" s="4" t="n"/>
-      <c r="L14" s="4" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -1199,8 +1169,6 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="n"/>
-      <c r="B16" s="3" t="n"/>
       <c r="C16" s="3" t="inlineStr">
         <is>
           <t>40</t>
@@ -1231,10 +1199,6 @@
           <t>.1200</t>
         </is>
       </c>
-      <c r="I16" s="3" t="n"/>
-      <c r="J16" s="3" t="n"/>
-      <c r="K16" s="3" t="n"/>
-      <c r="L16" s="3" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
@@ -1299,8 +1263,6 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="n"/>
-      <c r="B18" s="4" t="n"/>
       <c r="C18" s="4" t="inlineStr">
         <is>
           <t>36</t>
@@ -1331,10 +1293,6 @@
           <t>.1470</t>
         </is>
       </c>
-      <c r="I18" s="4" t="n"/>
-      <c r="J18" s="4" t="n"/>
-      <c r="K18" s="4" t="n"/>
-      <c r="L18" s="4" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
@@ -1399,8 +1357,6 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="n"/>
-      <c r="B20" s="3" t="n"/>
       <c r="C20" s="3" t="inlineStr">
         <is>
           <t>32</t>
@@ -1431,10 +1387,6 @@
           <t>.1695</t>
         </is>
       </c>
-      <c r="I20" s="3" t="n"/>
-      <c r="J20" s="3" t="n"/>
-      <c r="K20" s="3" t="n"/>
-      <c r="L20" s="3" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
@@ -1499,8 +1451,6 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="n"/>
-      <c r="B22" s="4" t="n"/>
       <c r="C22" s="4" t="inlineStr">
         <is>
           <t>28</t>
@@ -1531,14 +1481,8 @@
           <t>.1935</t>
         </is>
       </c>
-      <c r="I22" s="4" t="n"/>
-      <c r="J22" s="4" t="n"/>
-      <c r="K22" s="4" t="n"/>
-      <c r="L22" s="4" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="n"/>
-      <c r="B23" s="4" t="n"/>
       <c r="C23" s="4" t="inlineStr">
         <is>
           <t>32</t>
@@ -1569,10 +1513,6 @@
           <t>.1960</t>
         </is>
       </c>
-      <c r="I23" s="4" t="n"/>
-      <c r="J23" s="4" t="n"/>
-      <c r="K23" s="4" t="n"/>
-      <c r="L23" s="4" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
@@ -1637,8 +1577,6 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="n"/>
-      <c r="B25" s="3" t="n"/>
       <c r="C25" s="3" t="inlineStr">
         <is>
           <t>28</t>
@@ -1669,14 +1607,8 @@
           <t>.2280</t>
         </is>
       </c>
-      <c r="I25" s="3" t="n"/>
-      <c r="J25" s="3" t="n"/>
-      <c r="K25" s="3" t="n"/>
-      <c r="L25" s="3" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="n"/>
-      <c r="B26" s="3" t="n"/>
       <c r="C26" s="3" t="inlineStr">
         <is>
           <t>32</t>
@@ -1707,10 +1639,6 @@
           <t>.2280</t>
         </is>
       </c>
-      <c r="I26" s="3" t="n"/>
-      <c r="J26" s="3" t="n"/>
-      <c r="K26" s="3" t="n"/>
-      <c r="L26" s="3" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
@@ -1775,8 +1703,6 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="n"/>
-      <c r="B28" s="4" t="n"/>
       <c r="C28" s="4" t="inlineStr">
         <is>
           <t>24</t>
@@ -1807,14 +1733,8 @@
           <t>.2812</t>
         </is>
       </c>
-      <c r="I28" s="4" t="n"/>
-      <c r="J28" s="4" t="n"/>
-      <c r="K28" s="4" t="n"/>
-      <c r="L28" s="4" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="n"/>
-      <c r="B29" s="4" t="n"/>
       <c r="C29" s="4" t="inlineStr">
         <is>
           <t>32</t>
@@ -1845,10 +1765,6 @@
           <t>.2900</t>
         </is>
       </c>
-      <c r="I29" s="4" t="n"/>
-      <c r="J29" s="4" t="n"/>
-      <c r="K29" s="4" t="n"/>
-      <c r="L29" s="4" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
@@ -1913,8 +1829,6 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="n"/>
-      <c r="B31" s="3" t="n"/>
       <c r="C31" s="3" t="inlineStr">
         <is>
           <t>24</t>
@@ -1945,14 +1859,8 @@
           <t>.3480</t>
         </is>
       </c>
-      <c r="I31" s="3" t="n"/>
-      <c r="J31" s="3" t="n"/>
-      <c r="K31" s="3" t="n"/>
-      <c r="L31" s="3" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="n"/>
-      <c r="B32" s="3" t="n"/>
       <c r="C32" s="3" t="inlineStr">
         <is>
           <t>32</t>
@@ -1983,10 +1891,6 @@
           <t>.3580</t>
         </is>
       </c>
-      <c r="I32" s="3" t="n"/>
-      <c r="J32" s="3" t="n"/>
-      <c r="K32" s="3" t="n"/>
-      <c r="L32" s="3" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
@@ -2046,13 +1950,11 @@
       </c>
       <c r="L33" s="4" t="inlineStr">
         <is>
-          <t>.4687</t>
+          <t>.4688</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="n"/>
-      <c r="B34" s="4" t="n"/>
       <c r="C34" s="4" t="inlineStr">
         <is>
           <t>20</t>
@@ -2083,14 +1985,8 @@
           <t>.4062</t>
         </is>
       </c>
-      <c r="I34" s="4" t="n"/>
-      <c r="J34" s="4" t="n"/>
-      <c r="K34" s="4" t="n"/>
-      <c r="L34" s="4" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="n"/>
-      <c r="B35" s="4" t="n"/>
       <c r="C35" s="4" t="inlineStr">
         <is>
           <t>28</t>
@@ -2121,10 +2017,6 @@
           <t>.4130</t>
         </is>
       </c>
-      <c r="I35" s="4" t="n"/>
-      <c r="J35" s="4" t="n"/>
-      <c r="K35" s="4" t="n"/>
-      <c r="L35" s="4" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
@@ -2189,8 +2081,6 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="3" t="n"/>
-      <c r="B37" s="3" t="n"/>
       <c r="C37" s="3" t="inlineStr">
         <is>
           <t>20</t>
@@ -2221,14 +2111,8 @@
           <t>.4688</t>
         </is>
       </c>
-      <c r="I37" s="3" t="n"/>
-      <c r="J37" s="3" t="n"/>
-      <c r="K37" s="3" t="n"/>
-      <c r="L37" s="3" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="n"/>
-      <c r="B38" s="3" t="n"/>
       <c r="C38" s="3" t="inlineStr">
         <is>
           <t>28</t>
@@ -2259,10 +2143,6 @@
           <t>.4688</t>
         </is>
       </c>
-      <c r="I38" s="3" t="n"/>
-      <c r="J38" s="3" t="n"/>
-      <c r="K38" s="3" t="n"/>
-      <c r="L38" s="3" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
@@ -2327,8 +2207,6 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="n"/>
-      <c r="B40" s="4" t="n"/>
       <c r="C40" s="4" t="inlineStr">
         <is>
           <t>18</t>
@@ -2359,14 +2237,8 @@
           <t>.5312</t>
         </is>
       </c>
-      <c r="I40" s="4" t="n"/>
-      <c r="J40" s="4" t="n"/>
-      <c r="K40" s="4" t="n"/>
-      <c r="L40" s="4" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="n"/>
-      <c r="B41" s="4" t="n"/>
       <c r="C41" s="4" t="inlineStr">
         <is>
           <t>24</t>
@@ -2397,10 +2269,6 @@
           <t>.5312</t>
         </is>
       </c>
-      <c r="I41" s="4" t="n"/>
-      <c r="J41" s="4" t="n"/>
-      <c r="K41" s="4" t="n"/>
-      <c r="L41" s="4" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
@@ -2465,8 +2333,6 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="n"/>
-      <c r="B43" s="3" t="n"/>
       <c r="C43" s="3" t="inlineStr">
         <is>
           <t>18</t>
@@ -2497,14 +2363,8 @@
           <t>.5938</t>
         </is>
       </c>
-      <c r="I43" s="3" t="n"/>
-      <c r="J43" s="3" t="n"/>
-      <c r="K43" s="3" t="n"/>
-      <c r="L43" s="3" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="n"/>
-      <c r="B44" s="3" t="n"/>
       <c r="C44" s="3" t="inlineStr">
         <is>
           <t>24</t>
@@ -2535,10 +2395,6 @@
           <t>.5938</t>
         </is>
       </c>
-      <c r="I44" s="3" t="n"/>
-      <c r="J44" s="3" t="n"/>
-      <c r="K44" s="3" t="n"/>
-      <c r="L44" s="3" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
@@ -2665,8 +2521,6 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="n"/>
-      <c r="B47" s="3" t="n"/>
       <c r="C47" s="3" t="inlineStr">
         <is>
           <t>16</t>
@@ -2697,14 +2551,8 @@
           <t>.7031</t>
         </is>
       </c>
-      <c r="I47" s="3" t="n"/>
-      <c r="J47" s="3" t="n"/>
-      <c r="K47" s="3" t="n"/>
-      <c r="L47" s="3" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="3" t="n"/>
-      <c r="B48" s="3" t="n"/>
       <c r="C48" s="3" t="inlineStr">
         <is>
           <t>20</t>
@@ -2735,10 +2583,6 @@
           <t>.7188</t>
         </is>
       </c>
-      <c r="I48" s="3" t="n"/>
-      <c r="J48" s="3" t="n"/>
-      <c r="K48" s="3" t="n"/>
-      <c r="L48" s="3" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
@@ -2865,8 +2709,6 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="n"/>
-      <c r="B51" s="3" t="n"/>
       <c r="C51" s="3" t="inlineStr">
         <is>
           <t>14</t>
@@ -2897,14 +2739,8 @@
           <t>.8281</t>
         </is>
       </c>
-      <c r="I51" s="3" t="n"/>
-      <c r="J51" s="3" t="n"/>
-      <c r="K51" s="3" t="n"/>
-      <c r="L51" s="3" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="3" t="n"/>
-      <c r="B52" s="3" t="n"/>
       <c r="C52" s="3" t="inlineStr">
         <is>
           <t>20</t>
@@ -2935,10 +2771,6 @@
           <t>.8438</t>
         </is>
       </c>
-      <c r="I52" s="3" t="n"/>
-      <c r="J52" s="3" t="n"/>
-      <c r="K52" s="3" t="n"/>
-      <c r="L52" s="3" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="4" t="inlineStr">
@@ -3065,8 +2897,6 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="3" t="n"/>
-      <c r="B55" s="3" t="n"/>
       <c r="C55" s="3" t="inlineStr">
         <is>
           <t>12</t>
@@ -3097,14 +2927,8 @@
           <t>.9531</t>
         </is>
       </c>
-      <c r="I55" s="3" t="n"/>
-      <c r="J55" s="3" t="n"/>
-      <c r="K55" s="3" t="n"/>
-      <c r="L55" s="3" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="3" t="n"/>
-      <c r="B56" s="3" t="n"/>
       <c r="C56" s="3" t="inlineStr">
         <is>
           <t>20</t>
@@ -3135,10 +2959,6 @@
           <t>.9688</t>
         </is>
       </c>
-      <c r="I56" s="3" t="n"/>
-      <c r="J56" s="3" t="n"/>
-      <c r="K56" s="3" t="n"/>
-      <c r="L56" s="3" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="124">

</xml_diff>

<commit_message>
WIP large paper sizes
</commit_message>
<xml_diff>
--- a/inch_taps_drills.xlsx
+++ b/inch_taps_drills.xlsx
@@ -11876,7 +11876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:R56"/>
   <sheetViews>
@@ -11887,24 +11887,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
-    <col width="11" customWidth="1" min="15" max="15"/>
-    <col width="11" customWidth="1" min="16" max="16"/>
-    <col width="11" customWidth="1" min="17" max="17"/>
-    <col width="11" customWidth="1" min="18" max="18"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="27.5" customWidth="1" min="5" max="5"/>
+    <col width="27.5" customWidth="1" min="6" max="6"/>
+    <col width="27.5" customWidth="1" min="7" max="7"/>
+    <col width="27.5" customWidth="1" min="8" max="8"/>
+    <col width="27.5" customWidth="1" min="9" max="9"/>
+    <col width="27.5" customWidth="1" min="10" max="10"/>
+    <col width="27.5" customWidth="1" min="11" max="11"/>
+    <col width="27.5" customWidth="1" min="12" max="12"/>
+    <col width="27.5" customWidth="1" min="13" max="13"/>
+    <col width="27.5" customWidth="1" min="14" max="14"/>
+    <col width="27.5" customWidth="1" min="15" max="15"/>
+    <col width="27.5" customWidth="1" min="16" max="16"/>
+    <col width="27.5" customWidth="1" min="17" max="17"/>
+    <col width="27.5" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -15680,7 +15680,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="0" gridLines="0"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup orientation="landscape" paperSize="0" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup orientation="portrait" paperSize="0" paperHeight="24in" paperWidth="36in"/>
 </worksheet>
 </file>
 
@@ -15688,7 +15688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:R56"/>
   <sheetViews>
@@ -15699,24 +15699,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
-    <col width="11" customWidth="1" min="15" max="15"/>
-    <col width="11" customWidth="1" min="16" max="16"/>
-    <col width="11" customWidth="1" min="17" max="17"/>
-    <col width="11" customWidth="1" min="18" max="18"/>
+    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
+    <col width="38.5" customWidth="1" min="5" max="5"/>
+    <col width="38.5" customWidth="1" min="6" max="6"/>
+    <col width="38.5" customWidth="1" min="7" max="7"/>
+    <col width="38.5" customWidth="1" min="8" max="8"/>
+    <col width="38.5" customWidth="1" min="9" max="9"/>
+    <col width="38.5" customWidth="1" min="10" max="10"/>
+    <col width="38.5" customWidth="1" min="11" max="11"/>
+    <col width="38.5" customWidth="1" min="12" max="12"/>
+    <col width="38.5" customWidth="1" min="13" max="13"/>
+    <col width="38.5" customWidth="1" min="14" max="14"/>
+    <col width="38.5" customWidth="1" min="15" max="15"/>
+    <col width="38.5" customWidth="1" min="16" max="16"/>
+    <col width="38.5" customWidth="1" min="17" max="17"/>
+    <col width="38.5" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -19492,6 +19492,6 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="0" gridLines="0"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup orientation="landscape" paperSize="0" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup orientation="portrait" paperSize="0" paperHeight="36in" paperWidth="48in"/>
 </worksheet>
 </file>
</xml_diff>